<commit_message>
Sample file generated using new hour notation
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -95,55 +95,55 @@
     <t>21/06</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>05:00</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>22:00</t>
   </si>
 </sst>
 </file>

</xml_diff>